<commit_message>
Base con NMC, ln, y lags de datos comerciales
</commit_message>
<xml_diff>
--- a/data/versiones/base_china_v1_ref.xlsx
+++ b/data/versiones/base_china_v1_ref.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Proyecto China\Proyecto China\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diplomado CSC\proyecto-china\data\versiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4336EB33-93C3-493A-8ECD-905CEBB35D6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E209B053-6225-46F3-BE06-89F210A56456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0717F9F0-ADF3-4DD4-8CCE-67E692758DA8}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>